<commit_message>
Update full project 27/02/2015 16:35
</commit_message>
<xml_diff>
--- a/doc/backend/api/TRN-MiniBlog_API-Specification_TENHO.xlsx
+++ b/doc/backend/api/TRN-MiniBlog_API-Specification_TENHO.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER_MLD3\Desktop\miniblog\doc\backend\api\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14080" tabRatio="957" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14085" tabRatio="957" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="23" r:id="rId1"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="253">
   <si>
     <t>Description</t>
   </si>
@@ -849,16 +854,31 @@
       <t>ccount</t>
     </r>
   </si>
+  <si>
+    <t>Username already exist</t>
+  </si>
+  <si>
+    <t>Username or password is incorrect</t>
+  </si>
+  <si>
+    <t>Wrong password</t>
+  </si>
+  <si>
+    <t>Username is existed</t>
+  </si>
+  <si>
+    <t>Wrong username or password</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="36">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -866,7 +886,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -874,7 +894,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -882,7 +902,7 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -895,45 +915,45 @@
     <font>
       <sz val="18"/>
       <color theme="0"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="5" tint="-0.249977111117893"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF963634"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -948,7 +968,7 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2097,29 +2117,73 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="11" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="10" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="17" fillId="6" borderId="11" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="6" borderId="10" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="13" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="6" borderId="11" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -2131,44 +2195,6 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -2197,6 +2223,21 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="11" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="10" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -2209,48 +2250,30 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="17" fillId="6" borderId="11" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="6" borderId="11" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="17" fillId="6" borderId="10" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="13" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2260,9 +2283,6 @@
     <xf numFmtId="0" fontId="32" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2293,17 +2313,14 @@
     <xf numFmtId="49" fontId="13" fillId="8" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2322,20 +2339,23 @@
     <xf numFmtId="0" fontId="27" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="411">
@@ -4412,305 +4432,305 @@
       <selection activeCell="X10" sqref="X10:AC10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="70" width="4.83203125" style="44" customWidth="1"/>
-    <col min="71" max="95" width="3.6640625" style="44" customWidth="1"/>
-    <col min="96" max="16384" width="10.83203125" style="44"/>
+    <col min="1" max="70" width="4.875" style="44" customWidth="1"/>
+    <col min="71" max="95" width="3.625" style="44" customWidth="1"/>
+    <col min="96" max="16384" width="10.875" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="43" customFormat="1">
-      <c r="A1" s="158" t="s">
+    <row r="1" spans="1:30" s="43" customFormat="1" ht="15.75">
+      <c r="A1" s="189" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="161" t="s">
+      <c r="B1" s="190"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="192" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="162"/>
-      <c r="F1" s="162"/>
-      <c r="G1" s="162"/>
-      <c r="H1" s="162"/>
-      <c r="I1" s="162"/>
-      <c r="J1" s="162"/>
-      <c r="K1" s="163" t="s">
+      <c r="E1" s="193"/>
+      <c r="F1" s="193"/>
+      <c r="G1" s="193"/>
+      <c r="H1" s="193"/>
+      <c r="I1" s="193"/>
+      <c r="J1" s="193"/>
+      <c r="K1" s="197" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="164"/>
-      <c r="M1" s="165"/>
-      <c r="N1" s="166" t="s">
+      <c r="L1" s="198"/>
+      <c r="M1" s="199"/>
+      <c r="N1" s="179" t="s">
         <v>157</v>
       </c>
-      <c r="O1" s="167"/>
-      <c r="P1" s="167"/>
-      <c r="Q1" s="167"/>
-      <c r="R1" s="167"/>
-      <c r="S1" s="167"/>
-      <c r="T1" s="167"/>
-      <c r="U1" s="168"/>
-      <c r="V1" s="169" t="s">
+      <c r="O1" s="180"/>
+      <c r="P1" s="180"/>
+      <c r="Q1" s="180"/>
+      <c r="R1" s="180"/>
+      <c r="S1" s="180"/>
+      <c r="T1" s="180"/>
+      <c r="U1" s="181"/>
+      <c r="V1" s="200" t="s">
         <v>28</v>
       </c>
-      <c r="W1" s="170"/>
-      <c r="X1" s="170"/>
-      <c r="Y1" s="170"/>
-      <c r="Z1" s="170"/>
-      <c r="AA1" s="170"/>
-      <c r="AB1" s="170"/>
-      <c r="AC1" s="170"/>
-      <c r="AD1" s="171"/>
-    </row>
-    <row r="2" spans="1:30" s="43" customFormat="1">
-      <c r="A2" s="158" t="s">
+      <c r="W1" s="201"/>
+      <c r="X1" s="201"/>
+      <c r="Y1" s="201"/>
+      <c r="Z1" s="201"/>
+      <c r="AA1" s="201"/>
+      <c r="AB1" s="201"/>
+      <c r="AC1" s="201"/>
+      <c r="AD1" s="202"/>
+    </row>
+    <row r="2" spans="1:30" s="43" customFormat="1" ht="15.75">
+      <c r="A2" s="189" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="159"/>
-      <c r="C2" s="160"/>
-      <c r="D2" s="161" t="s">
+      <c r="B2" s="190"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="192" t="s">
         <v>160</v>
       </c>
-      <c r="E2" s="162"/>
-      <c r="F2" s="162"/>
-      <c r="G2" s="162"/>
-      <c r="H2" s="162"/>
-      <c r="I2" s="162"/>
-      <c r="J2" s="162"/>
-      <c r="K2" s="175" t="s">
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="193"/>
+      <c r="I2" s="193"/>
+      <c r="J2" s="193"/>
+      <c r="K2" s="174" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="176"/>
-      <c r="M2" s="177"/>
-      <c r="N2" s="187" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="176"/>
+      <c r="N2" s="194" t="s">
         <v>162</v>
       </c>
-      <c r="O2" s="188"/>
-      <c r="P2" s="188"/>
-      <c r="Q2" s="188"/>
-      <c r="R2" s="188"/>
-      <c r="S2" s="188"/>
-      <c r="T2" s="188"/>
-      <c r="U2" s="189"/>
-      <c r="V2" s="172" t="s">
+      <c r="O2" s="195"/>
+      <c r="P2" s="195"/>
+      <c r="Q2" s="195"/>
+      <c r="R2" s="195"/>
+      <c r="S2" s="195"/>
+      <c r="T2" s="195"/>
+      <c r="U2" s="196"/>
+      <c r="V2" s="171" t="s">
         <v>164</v>
       </c>
-      <c r="W2" s="173"/>
-      <c r="X2" s="174"/>
-      <c r="Y2" s="172" t="s">
+      <c r="W2" s="172"/>
+      <c r="X2" s="173"/>
+      <c r="Y2" s="171" t="s">
         <v>31</v>
       </c>
-      <c r="Z2" s="173"/>
-      <c r="AA2" s="174"/>
-      <c r="AB2" s="172" t="s">
+      <c r="Z2" s="172"/>
+      <c r="AA2" s="173"/>
+      <c r="AB2" s="171" t="s">
         <v>32</v>
       </c>
-      <c r="AC2" s="173"/>
-      <c r="AD2" s="174"/>
-    </row>
-    <row r="3" spans="1:30" s="43" customFormat="1">
-      <c r="A3" s="175" t="s">
+      <c r="AC2" s="172"/>
+      <c r="AD2" s="173"/>
+    </row>
+    <row r="3" spans="1:30" s="43" customFormat="1" ht="15.75">
+      <c r="A3" s="174" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="176"/>
-      <c r="C3" s="177"/>
-      <c r="D3" s="178" t="s">
+      <c r="B3" s="175"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="177" t="s">
         <v>161</v>
       </c>
-      <c r="E3" s="179"/>
-      <c r="F3" s="179"/>
-      <c r="G3" s="179"/>
-      <c r="H3" s="179"/>
-      <c r="I3" s="179"/>
-      <c r="J3" s="179"/>
-      <c r="K3" s="175" t="s">
+      <c r="E3" s="178"/>
+      <c r="F3" s="178"/>
+      <c r="G3" s="178"/>
+      <c r="H3" s="178"/>
+      <c r="I3" s="178"/>
+      <c r="J3" s="178"/>
+      <c r="K3" s="174" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="176"/>
-      <c r="M3" s="177"/>
-      <c r="N3" s="166" t="s">
+      <c r="L3" s="175"/>
+      <c r="M3" s="176"/>
+      <c r="N3" s="179" t="s">
         <v>163</v>
       </c>
-      <c r="O3" s="167"/>
-      <c r="P3" s="167"/>
-      <c r="Q3" s="167"/>
-      <c r="R3" s="167"/>
-      <c r="S3" s="167"/>
-      <c r="T3" s="167"/>
-      <c r="U3" s="168"/>
-      <c r="V3" s="180"/>
-      <c r="W3" s="181"/>
-      <c r="X3" s="182"/>
-      <c r="Y3" s="183"/>
-      <c r="Z3" s="184"/>
-      <c r="AA3" s="185"/>
-      <c r="AB3" s="186"/>
-      <c r="AC3" s="184"/>
-      <c r="AD3" s="185"/>
-    </row>
-    <row r="7" spans="1:30" ht="16" thickBot="1"/>
-    <row r="8" spans="1:30" ht="16" thickBot="1">
-      <c r="B8" s="202" t="s">
+      <c r="O3" s="180"/>
+      <c r="P3" s="180"/>
+      <c r="Q3" s="180"/>
+      <c r="R3" s="180"/>
+      <c r="S3" s="180"/>
+      <c r="T3" s="180"/>
+      <c r="U3" s="181"/>
+      <c r="V3" s="182"/>
+      <c r="W3" s="183"/>
+      <c r="X3" s="184"/>
+      <c r="Y3" s="185"/>
+      <c r="Z3" s="186"/>
+      <c r="AA3" s="187"/>
+      <c r="AB3" s="188"/>
+      <c r="AC3" s="186"/>
+      <c r="AD3" s="187"/>
+    </row>
+    <row r="7" spans="1:30" ht="15.75" thickBot="1"/>
+    <row r="8" spans="1:30" ht="16.5" thickBot="1">
+      <c r="B8" s="169" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="202"/>
-      <c r="D8" s="202"/>
-      <c r="E8" s="202"/>
-      <c r="F8" s="202" t="s">
+      <c r="C8" s="169"/>
+      <c r="D8" s="169"/>
+      <c r="E8" s="169"/>
+      <c r="F8" s="169" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="202"/>
-      <c r="H8" s="202" t="s">
+      <c r="G8" s="169"/>
+      <c r="H8" s="169" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="202"/>
-      <c r="J8" s="202"/>
-      <c r="K8" s="202" t="s">
+      <c r="I8" s="169"/>
+      <c r="J8" s="169"/>
+      <c r="K8" s="169" t="s">
         <v>0</v>
       </c>
-      <c r="L8" s="202"/>
-      <c r="M8" s="202"/>
-      <c r="N8" s="202"/>
-      <c r="O8" s="202"/>
-      <c r="P8" s="202"/>
-      <c r="Q8" s="202"/>
-      <c r="R8" s="202"/>
-      <c r="S8" s="202"/>
-      <c r="T8" s="202"/>
-      <c r="U8" s="202"/>
-      <c r="V8" s="202"/>
-      <c r="W8" s="202"/>
-      <c r="X8" s="202" t="s">
+      <c r="L8" s="169"/>
+      <c r="M8" s="169"/>
+      <c r="N8" s="169"/>
+      <c r="O8" s="169"/>
+      <c r="P8" s="169"/>
+      <c r="Q8" s="169"/>
+      <c r="R8" s="169"/>
+      <c r="S8" s="169"/>
+      <c r="T8" s="169"/>
+      <c r="U8" s="169"/>
+      <c r="V8" s="169"/>
+      <c r="W8" s="169"/>
+      <c r="X8" s="169" t="s">
         <v>36</v>
       </c>
-      <c r="Y8" s="202"/>
-      <c r="Z8" s="202"/>
-      <c r="AA8" s="202"/>
-      <c r="AB8" s="202"/>
-      <c r="AC8" s="202"/>
+      <c r="Y8" s="169"/>
+      <c r="Z8" s="169"/>
+      <c r="AA8" s="169"/>
+      <c r="AB8" s="169"/>
+      <c r="AC8" s="169"/>
     </row>
     <row r="9" spans="1:30">
-      <c r="B9" s="190" t="s">
+      <c r="B9" s="170" t="s">
         <v>159</v>
       </c>
-      <c r="C9" s="191"/>
-      <c r="D9" s="191"/>
-      <c r="E9" s="192"/>
-      <c r="F9" s="193" t="s">
+      <c r="C9" s="159"/>
+      <c r="D9" s="159"/>
+      <c r="E9" s="160"/>
+      <c r="F9" s="161" t="s">
         <v>156</v>
       </c>
-      <c r="G9" s="194"/>
-      <c r="H9" s="195"/>
-      <c r="I9" s="191"/>
-      <c r="J9" s="192"/>
-      <c r="K9" s="196"/>
-      <c r="L9" s="197"/>
-      <c r="M9" s="197"/>
-      <c r="N9" s="197"/>
-      <c r="O9" s="197"/>
-      <c r="P9" s="197"/>
-      <c r="Q9" s="197"/>
-      <c r="R9" s="197"/>
-      <c r="S9" s="197"/>
-      <c r="T9" s="197"/>
-      <c r="U9" s="197"/>
-      <c r="V9" s="197"/>
-      <c r="W9" s="198"/>
-      <c r="X9" s="199"/>
-      <c r="Y9" s="200"/>
-      <c r="Z9" s="200"/>
-      <c r="AA9" s="200"/>
-      <c r="AB9" s="200"/>
-      <c r="AC9" s="201"/>
+      <c r="G9" s="162"/>
+      <c r="H9" s="158"/>
+      <c r="I9" s="159"/>
+      <c r="J9" s="160"/>
+      <c r="K9" s="163"/>
+      <c r="L9" s="164"/>
+      <c r="M9" s="164"/>
+      <c r="N9" s="164"/>
+      <c r="O9" s="164"/>
+      <c r="P9" s="164"/>
+      <c r="Q9" s="164"/>
+      <c r="R9" s="164"/>
+      <c r="S9" s="164"/>
+      <c r="T9" s="164"/>
+      <c r="U9" s="164"/>
+      <c r="V9" s="164"/>
+      <c r="W9" s="165"/>
+      <c r="X9" s="166"/>
+      <c r="Y9" s="167"/>
+      <c r="Z9" s="167"/>
+      <c r="AA9" s="167"/>
+      <c r="AB9" s="167"/>
+      <c r="AC9" s="168"/>
     </row>
     <row r="10" spans="1:30">
-      <c r="B10" s="195"/>
-      <c r="C10" s="191"/>
-      <c r="D10" s="191"/>
-      <c r="E10" s="192"/>
-      <c r="F10" s="193"/>
-      <c r="G10" s="194"/>
-      <c r="H10" s="195"/>
-      <c r="I10" s="191"/>
-      <c r="J10" s="192"/>
-      <c r="K10" s="196"/>
-      <c r="L10" s="197"/>
-      <c r="M10" s="197"/>
-      <c r="N10" s="197"/>
-      <c r="O10" s="197"/>
-      <c r="P10" s="197"/>
-      <c r="Q10" s="197"/>
-      <c r="R10" s="197"/>
-      <c r="S10" s="197"/>
-      <c r="T10" s="197"/>
-      <c r="U10" s="197"/>
-      <c r="V10" s="197"/>
-      <c r="W10" s="198"/>
-      <c r="X10" s="199"/>
-      <c r="Y10" s="200"/>
-      <c r="Z10" s="200"/>
-      <c r="AA10" s="200"/>
-      <c r="AB10" s="200"/>
-      <c r="AC10" s="201"/>
+      <c r="B10" s="158"/>
+      <c r="C10" s="159"/>
+      <c r="D10" s="159"/>
+      <c r="E10" s="160"/>
+      <c r="F10" s="161"/>
+      <c r="G10" s="162"/>
+      <c r="H10" s="158"/>
+      <c r="I10" s="159"/>
+      <c r="J10" s="160"/>
+      <c r="K10" s="163"/>
+      <c r="L10" s="164"/>
+      <c r="M10" s="164"/>
+      <c r="N10" s="164"/>
+      <c r="O10" s="164"/>
+      <c r="P10" s="164"/>
+      <c r="Q10" s="164"/>
+      <c r="R10" s="164"/>
+      <c r="S10" s="164"/>
+      <c r="T10" s="164"/>
+      <c r="U10" s="164"/>
+      <c r="V10" s="164"/>
+      <c r="W10" s="165"/>
+      <c r="X10" s="166"/>
+      <c r="Y10" s="167"/>
+      <c r="Z10" s="167"/>
+      <c r="AA10" s="167"/>
+      <c r="AB10" s="167"/>
+      <c r="AC10" s="168"/>
     </row>
     <row r="11" spans="1:30">
-      <c r="B11" s="195"/>
-      <c r="C11" s="191"/>
-      <c r="D11" s="191"/>
-      <c r="E11" s="192"/>
-      <c r="F11" s="193"/>
-      <c r="G11" s="194"/>
-      <c r="H11" s="195"/>
-      <c r="I11" s="191"/>
-      <c r="J11" s="192"/>
-      <c r="K11" s="196"/>
-      <c r="L11" s="197"/>
-      <c r="M11" s="197"/>
-      <c r="N11" s="197"/>
-      <c r="O11" s="197"/>
-      <c r="P11" s="197"/>
-      <c r="Q11" s="197"/>
-      <c r="R11" s="197"/>
-      <c r="S11" s="197"/>
-      <c r="T11" s="197"/>
-      <c r="U11" s="197"/>
-      <c r="V11" s="197"/>
-      <c r="W11" s="198"/>
-      <c r="X11" s="199"/>
-      <c r="Y11" s="200"/>
-      <c r="Z11" s="200"/>
-      <c r="AA11" s="200"/>
-      <c r="AB11" s="200"/>
-      <c r="AC11" s="201"/>
+      <c r="B11" s="158"/>
+      <c r="C11" s="159"/>
+      <c r="D11" s="159"/>
+      <c r="E11" s="160"/>
+      <c r="F11" s="161"/>
+      <c r="G11" s="162"/>
+      <c r="H11" s="158"/>
+      <c r="I11" s="159"/>
+      <c r="J11" s="160"/>
+      <c r="K11" s="163"/>
+      <c r="L11" s="164"/>
+      <c r="M11" s="164"/>
+      <c r="N11" s="164"/>
+      <c r="O11" s="164"/>
+      <c r="P11" s="164"/>
+      <c r="Q11" s="164"/>
+      <c r="R11" s="164"/>
+      <c r="S11" s="164"/>
+      <c r="T11" s="164"/>
+      <c r="U11" s="164"/>
+      <c r="V11" s="164"/>
+      <c r="W11" s="165"/>
+      <c r="X11" s="166"/>
+      <c r="Y11" s="167"/>
+      <c r="Z11" s="167"/>
+      <c r="AA11" s="167"/>
+      <c r="AB11" s="167"/>
+      <c r="AC11" s="168"/>
     </row>
     <row r="12" spans="1:30">
-      <c r="B12" s="195"/>
-      <c r="C12" s="191"/>
-      <c r="D12" s="191"/>
-      <c r="E12" s="192"/>
-      <c r="F12" s="193"/>
-      <c r="G12" s="194"/>
-      <c r="H12" s="195"/>
-      <c r="I12" s="191"/>
-      <c r="J12" s="192"/>
-      <c r="K12" s="196"/>
-      <c r="L12" s="197"/>
-      <c r="M12" s="197"/>
-      <c r="N12" s="197"/>
-      <c r="O12" s="197"/>
-      <c r="P12" s="197"/>
-      <c r="Q12" s="197"/>
-      <c r="R12" s="197"/>
-      <c r="S12" s="197"/>
-      <c r="T12" s="197"/>
-      <c r="U12" s="197"/>
-      <c r="V12" s="197"/>
-      <c r="W12" s="198"/>
-      <c r="X12" s="199"/>
-      <c r="Y12" s="200"/>
-      <c r="Z12" s="200"/>
-      <c r="AA12" s="200"/>
-      <c r="AB12" s="200"/>
-      <c r="AC12" s="201"/>
+      <c r="B12" s="158"/>
+      <c r="C12" s="159"/>
+      <c r="D12" s="159"/>
+      <c r="E12" s="160"/>
+      <c r="F12" s="161"/>
+      <c r="G12" s="162"/>
+      <c r="H12" s="158"/>
+      <c r="I12" s="159"/>
+      <c r="J12" s="160"/>
+      <c r="K12" s="163"/>
+      <c r="L12" s="164"/>
+      <c r="M12" s="164"/>
+      <c r="N12" s="164"/>
+      <c r="O12" s="164"/>
+      <c r="P12" s="164"/>
+      <c r="Q12" s="164"/>
+      <c r="R12" s="164"/>
+      <c r="S12" s="164"/>
+      <c r="T12" s="164"/>
+      <c r="U12" s="164"/>
+      <c r="V12" s="164"/>
+      <c r="W12" s="165"/>
+      <c r="X12" s="166"/>
+      <c r="Y12" s="167"/>
+      <c r="Z12" s="167"/>
+      <c r="AA12" s="167"/>
+      <c r="AB12" s="167"/>
+      <c r="AC12" s="168"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1"/>
     <row r="14" spans="1:30" ht="18" customHeight="1"/>
@@ -4740,31 +4760,11 @@
     <row r="38" ht="18" customHeight="1"/>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:W12"/>
-    <mergeCell ref="X12:AC12"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:W10"/>
-    <mergeCell ref="X10:AC10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="K11:W11"/>
-    <mergeCell ref="X11:AC11"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:W8"/>
-    <mergeCell ref="X8:AC8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K9:W9"/>
-    <mergeCell ref="X9:AC9"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:AD1"/>
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="AB2:AD2"/>
     <mergeCell ref="A3:C3"/>
@@ -4779,11 +4779,31 @@
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="N2:U2"/>
     <mergeCell ref="V2:X2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:AD1"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:W9"/>
+    <mergeCell ref="X9:AC9"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:W8"/>
+    <mergeCell ref="X8:AC8"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="K11:W11"/>
+    <mergeCell ref="X11:AC11"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:W10"/>
+    <mergeCell ref="X10:AC10"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:W12"/>
+    <mergeCell ref="X12:AC12"/>
   </mergeCells>
   <phoneticPr fontId="14"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4804,17 +4824,17 @@
       <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="10.83203125" style="2"/>
+    <col min="1" max="2" width="10.875" style="1"/>
+    <col min="3" max="3" width="10.875" style="2"/>
     <col min="4" max="4" width="53" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="52.5" style="30" customWidth="1"/>
-    <col min="6" max="6" width="52.33203125" style="30" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="52.375" style="30" customWidth="1"/>
+    <col min="7" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="3" customFormat="1" ht="26" customHeight="1">
+    <row r="1" spans="2:6" s="3" customFormat="1" ht="26.1" customHeight="1">
       <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
@@ -4825,7 +4845,7 @@
     <row r="3" spans="2:6">
       <c r="E3" s="23"/>
     </row>
-    <row r="4" spans="2:6" ht="20">
+    <row r="4" spans="2:6" ht="18.75">
       <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
@@ -4833,7 +4853,7 @@
       <c r="E4" s="24"/>
       <c r="F4" s="24"/>
     </row>
-    <row r="5" spans="2:6" ht="20">
+    <row r="5" spans="2:6" ht="18.75">
       <c r="C5" s="7" t="s">
         <v>39</v>
       </c>
@@ -4841,7 +4861,7 @@
       <c r="E5" s="24"/>
       <c r="F5" s="24"/>
     </row>
-    <row r="6" spans="2:6" ht="20">
+    <row r="6" spans="2:6" ht="18.75">
       <c r="C6" s="8" t="s">
         <v>24</v>
       </c>
@@ -4855,7 +4875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="20">
+    <row r="7" spans="2:6" ht="18.75">
       <c r="C7" s="7">
         <v>1</v>
       </c>
@@ -4869,7 +4889,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="20">
+    <row r="8" spans="2:6" ht="18.75">
       <c r="C8" s="7">
         <v>2</v>
       </c>
@@ -4883,19 +4903,19 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="20">
+    <row r="9" spans="2:6" ht="18.75">
       <c r="C9" s="7"/>
       <c r="D9" s="11"/>
       <c r="E9" s="27"/>
       <c r="F9" s="27"/>
     </row>
-    <row r="10" spans="2:6" ht="20">
+    <row r="10" spans="2:6" ht="18.75">
       <c r="C10" s="7"/>
       <c r="D10" s="12"/>
       <c r="E10" s="27"/>
       <c r="F10" s="27"/>
     </row>
-    <row r="11" spans="2:6" ht="20">
+    <row r="11" spans="2:6" ht="18.75">
       <c r="C11" s="13" t="s">
         <v>45</v>
       </c>
@@ -4903,7 +4923,7 @@
       <c r="E11" s="27"/>
       <c r="F11" s="27"/>
     </row>
-    <row r="12" spans="2:6" ht="20">
+    <row r="12" spans="2:6" ht="18.75">
       <c r="C12" s="14" t="s">
         <v>46</v>
       </c>
@@ -4911,7 +4931,7 @@
       <c r="E12" s="27"/>
       <c r="F12" s="27"/>
     </row>
-    <row r="13" spans="2:6" ht="20">
+    <row r="13" spans="2:6" ht="18.75">
       <c r="C13" s="8" t="s">
         <v>24</v>
       </c>
@@ -4925,7 +4945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="20">
+    <row r="14" spans="2:6" ht="18.75">
       <c r="C14" s="7">
         <v>1</v>
       </c>
@@ -4939,7 +4959,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="20">
+    <row r="15" spans="2:6" ht="18.75">
       <c r="C15" s="7">
         <v>2</v>
       </c>
@@ -4953,7 +4973,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="20">
+    <row r="16" spans="2:6" ht="18.75">
       <c r="C16" s="7">
         <v>3</v>
       </c>
@@ -4967,13 +4987,13 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="3:6" ht="20">
+    <row r="17" spans="3:6" ht="18.75">
       <c r="C17" s="7"/>
       <c r="D17" s="6"/>
       <c r="E17" s="24"/>
       <c r="F17" s="24"/>
     </row>
-    <row r="18" spans="3:6" ht="20">
+    <row r="18" spans="3:6" ht="18.75">
       <c r="C18" s="15" t="s">
         <v>50</v>
       </c>
@@ -4981,7 +5001,7 @@
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
     </row>
-    <row r="19" spans="3:6" ht="20">
+    <row r="19" spans="3:6" ht="18.75">
       <c r="C19" s="17" t="s">
         <v>51</v>
       </c>
@@ -4989,7 +5009,7 @@
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
     </row>
-    <row r="20" spans="3:6" ht="20">
+    <row r="20" spans="3:6" ht="18.75">
       <c r="C20" s="18" t="s">
         <v>24</v>
       </c>
@@ -5003,7 +5023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:6" ht="20">
+    <row r="21" spans="3:6" ht="18.75">
       <c r="C21" s="20">
         <v>1</v>
       </c>
@@ -5017,7 +5037,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="3:6" ht="20">
+    <row r="22" spans="3:6" ht="18.75">
       <c r="C22" s="20">
         <v>2</v>
       </c>
@@ -5031,7 +5051,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="3:6" ht="20">
+    <row r="23" spans="3:6" ht="18.75">
       <c r="C23" s="20">
         <v>3</v>
       </c>
@@ -5045,7 +5065,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="3:6" ht="20">
+    <row r="24" spans="3:6" ht="18.75">
       <c r="C24" s="20">
         <v>4</v>
       </c>
@@ -5059,7 +5079,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="3:6" ht="20">
+    <row r="25" spans="3:6" ht="18.75">
       <c r="C25" s="20">
         <v>5</v>
       </c>
@@ -5073,7 +5093,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="3:6" ht="20">
+    <row r="28" spans="3:6" ht="18.75">
       <c r="C28" s="15" t="s">
         <v>72</v>
       </c>
@@ -5081,7 +5101,7 @@
       <c r="E28" s="28"/>
       <c r="F28" s="28"/>
     </row>
-    <row r="29" spans="3:6" ht="20">
+    <row r="29" spans="3:6" ht="18.75">
       <c r="C29" s="17" t="s">
         <v>74</v>
       </c>
@@ -5089,7 +5109,7 @@
       <c r="E29" s="28"/>
       <c r="F29" s="28"/>
     </row>
-    <row r="30" spans="3:6" ht="20">
+    <row r="30" spans="3:6" ht="18.75">
       <c r="C30" s="18" t="s">
         <v>24</v>
       </c>
@@ -5103,7 +5123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="3:6" ht="20">
+    <row r="31" spans="3:6" ht="18.75">
       <c r="C31" s="20">
         <v>1</v>
       </c>
@@ -5117,7 +5137,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="3:6" ht="20">
+    <row r="32" spans="3:6" ht="18.75">
       <c r="C32" s="20">
         <v>2</v>
       </c>
@@ -5131,19 +5151,19 @@
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="3:6" ht="20">
+    <row r="33" spans="3:6" ht="18.75">
       <c r="C33" s="20"/>
       <c r="D33" s="21"/>
       <c r="E33" s="26"/>
       <c r="F33" s="32"/>
     </row>
-    <row r="34" spans="3:6" ht="20">
+    <row r="34" spans="3:6" ht="18.75">
       <c r="C34" s="20"/>
       <c r="D34" s="21"/>
       <c r="E34" s="26"/>
       <c r="F34" s="32"/>
     </row>
-    <row r="35" spans="3:6" ht="20">
+    <row r="35" spans="3:6" ht="18.75">
       <c r="C35" s="15" t="s">
         <v>67</v>
       </c>
@@ -5151,7 +5171,7 @@
       <c r="E35" s="28"/>
       <c r="F35" s="28"/>
     </row>
-    <row r="36" spans="3:6" ht="20">
+    <row r="36" spans="3:6" ht="18.75">
       <c r="C36" s="17" t="s">
         <v>68</v>
       </c>
@@ -5159,7 +5179,7 @@
       <c r="E36" s="28"/>
       <c r="F36" s="28"/>
     </row>
-    <row r="37" spans="3:6" ht="20">
+    <row r="37" spans="3:6" ht="18.75">
       <c r="C37" s="18" t="s">
         <v>24</v>
       </c>
@@ -5173,7 +5193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:6" ht="20">
+    <row r="38" spans="3:6" ht="18.75">
       <c r="C38" s="20">
         <v>1</v>
       </c>
@@ -5187,7 +5207,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="3:6" ht="20">
+    <row r="39" spans="3:6" ht="18.75">
       <c r="C39" s="20">
         <v>2</v>
       </c>
@@ -5201,7 +5221,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="3:6" ht="20">
+    <row r="40" spans="3:6" ht="18.75">
       <c r="C40" s="20">
         <v>3</v>
       </c>
@@ -5215,7 +5235,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="3:6" ht="20">
+    <row r="43" spans="3:6" ht="18.75">
       <c r="C43" s="15" t="s">
         <v>61</v>
       </c>
@@ -5223,7 +5243,7 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
     </row>
-    <row r="44" spans="3:6" ht="20">
+    <row r="44" spans="3:6" ht="18.75">
       <c r="C44" s="17" t="s">
         <v>60</v>
       </c>
@@ -5231,7 +5251,7 @@
       <c r="E44" s="28"/>
       <c r="F44" s="28"/>
     </row>
-    <row r="45" spans="3:6" ht="20">
+    <row r="45" spans="3:6" ht="18.75">
       <c r="C45" s="18" t="s">
         <v>24</v>
       </c>
@@ -5245,7 +5265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:6" ht="20">
+    <row r="46" spans="3:6" ht="18.75">
       <c r="C46" s="20">
         <v>1</v>
       </c>
@@ -5259,7 +5279,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="3:6" ht="20">
+    <row r="47" spans="3:6" ht="18.75">
       <c r="C47" s="20">
         <v>2</v>
       </c>
@@ -5273,7 +5293,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="50" spans="3:6" ht="20">
+    <row r="50" spans="3:6" ht="18.75">
       <c r="C50" s="15" t="s">
         <v>62</v>
       </c>
@@ -5281,7 +5301,7 @@
       <c r="E50" s="28"/>
       <c r="F50" s="28"/>
     </row>
-    <row r="51" spans="3:6" ht="20">
+    <row r="51" spans="3:6" ht="18.75">
       <c r="C51" s="17" t="s">
         <v>63</v>
       </c>
@@ -5289,7 +5309,7 @@
       <c r="E51" s="28"/>
       <c r="F51" s="28"/>
     </row>
-    <row r="52" spans="3:6" ht="20">
+    <row r="52" spans="3:6" ht="18.75">
       <c r="C52" s="18" t="s">
         <v>24</v>
       </c>
@@ -5303,7 +5323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="3:6" ht="20">
+    <row r="53" spans="3:6" ht="18.75">
       <c r="C53" s="20">
         <v>1</v>
       </c>
@@ -5317,7 +5337,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="3:6" ht="20">
+    <row r="56" spans="3:6" ht="18.75">
       <c r="C56" s="15" t="s">
         <v>123</v>
       </c>
@@ -5325,7 +5345,7 @@
       <c r="E56" s="28"/>
       <c r="F56" s="28"/>
     </row>
-    <row r="57" spans="3:6" ht="20">
+    <row r="57" spans="3:6" ht="18.75">
       <c r="C57" s="17" t="s">
         <v>124</v>
       </c>
@@ -5333,7 +5353,7 @@
       <c r="E57" s="28"/>
       <c r="F57" s="28"/>
     </row>
-    <row r="58" spans="3:6" ht="20">
+    <row r="58" spans="3:6" ht="18.75">
       <c r="C58" s="18" t="s">
         <v>24</v>
       </c>
@@ -5347,7 +5367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="3:6" ht="20">
+    <row r="59" spans="3:6" ht="18.75">
       <c r="C59" s="20">
         <v>1</v>
       </c>
@@ -5402,14 +5422,14 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="44"/>
-    <col min="3" max="3" width="5.33203125" style="44" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="44"/>
+    <col min="1" max="2" width="10.875" style="44"/>
+    <col min="3" max="3" width="5.375" style="44" customWidth="1"/>
+    <col min="4" max="16384" width="10.875" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="135" customFormat="1" ht="26" customHeight="1">
+    <row r="1" spans="2:11" s="135" customFormat="1" ht="26.1" customHeight="1">
       <c r="B1" s="56" t="s">
         <v>158</v>
       </c>
@@ -5427,7 +5447,7 @@
       <c r="J3" s="46"/>
       <c r="K3" s="47"/>
     </row>
-    <row r="4" spans="2:11">
+    <row r="4" spans="2:11" ht="15.75">
       <c r="B4" s="48"/>
       <c r="C4" s="136" t="s">
         <v>165</v>
@@ -5633,7 +5653,7 @@
       <c r="J20" s="49"/>
       <c r="K20" s="50"/>
     </row>
-    <row r="21" spans="2:14">
+    <row r="21" spans="2:14" ht="15.75">
       <c r="B21" s="48"/>
       <c r="C21" s="136" t="s">
         <v>166</v>
@@ -5833,23 +5853,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="36"/>
-    <col min="2" max="2" width="7.83203125" style="36" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="36" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" style="36" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" style="36" customWidth="1"/>
-    <col min="6" max="6" width="41.83203125" style="36" customWidth="1"/>
-    <col min="7" max="7" width="56.1640625" style="36" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="36"/>
+    <col min="1" max="1" width="10.875" style="36"/>
+    <col min="2" max="2" width="7.875" style="36" customWidth="1"/>
+    <col min="3" max="3" width="13.125" style="36" customWidth="1"/>
+    <col min="4" max="4" width="16.125" style="36" customWidth="1"/>
+    <col min="5" max="5" width="42.625" style="36" customWidth="1"/>
+    <col min="6" max="6" width="41.875" style="36" customWidth="1"/>
+    <col min="7" max="7" width="56.125" style="36" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" s="120" customFormat="1" ht="26" customHeight="1">
+    <row r="1" spans="2:12" s="120" customFormat="1" ht="26.1" customHeight="1">
       <c r="B1" s="133" t="s">
         <v>1</v>
       </c>
@@ -5867,7 +5887,7 @@
       <c r="K2" s="122"/>
       <c r="L2" s="122"/>
     </row>
-    <row r="3" spans="2:12">
+    <row r="3" spans="2:12" ht="15.75">
       <c r="B3" s="123" t="s">
         <v>20</v>
       </c>
@@ -5881,17 +5901,17 @@
       <c r="K3" s="122"/>
       <c r="L3" s="122"/>
     </row>
-    <row r="4" spans="2:12">
+    <row r="4" spans="2:12" ht="15.75">
       <c r="B4" s="104" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="104" t="s">
         <v>231</v>
       </c>
-      <c r="D4" s="204" t="s">
+      <c r="D4" s="205" t="s">
         <v>234</v>
       </c>
-      <c r="E4" s="204"/>
+      <c r="E4" s="205"/>
       <c r="F4" s="144" t="s">
         <v>232</v>
       </c>
@@ -5902,17 +5922,17 @@
       <c r="K4" s="122"/>
       <c r="L4" s="122"/>
     </row>
-    <row r="5" spans="2:12" ht="20" customHeight="1">
+    <row r="5" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B5" s="147">
         <v>1</v>
       </c>
       <c r="C5" s="148" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="207" t="s">
+      <c r="D5" s="204" t="s">
         <v>236</v>
       </c>
-      <c r="E5" s="207"/>
+      <c r="E5" s="204"/>
       <c r="F5" s="149" t="s">
         <v>235</v>
       </c>
@@ -5945,7 +5965,7 @@
       <c r="K7" s="122"/>
       <c r="L7" s="122"/>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8" spans="2:12" ht="15.75">
       <c r="B8" s="123" t="s">
         <v>3</v>
       </c>
@@ -5960,22 +5980,22 @@
       <c r="K8" s="122"/>
       <c r="L8" s="122"/>
     </row>
-    <row r="9" spans="2:12">
+    <row r="9" spans="2:12" ht="15.75">
       <c r="B9" s="104" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="144" t="s">
         <v>231</v>
       </c>
-      <c r="D9" s="204" t="s">
+      <c r="D9" s="205" t="s">
         <v>234</v>
       </c>
-      <c r="E9" s="204"/>
+      <c r="E9" s="205"/>
       <c r="F9" s="144" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="20" customHeight="1">
+    <row r="10" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B10" s="126">
         <v>1</v>
       </c>
@@ -5988,7 +6008,7 @@
       <c r="G10" s="125"/>
       <c r="H10" s="125"/>
     </row>
-    <row r="11" spans="2:12" ht="20" customHeight="1">
+    <row r="11" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B11" s="126">
         <v>2</v>
       </c>
@@ -6001,7 +6021,7 @@
       <c r="G11" s="125"/>
       <c r="H11" s="125"/>
     </row>
-    <row r="12" spans="2:12" ht="20" customHeight="1">
+    <row r="12" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B12" s="126">
         <v>3</v>
       </c>
@@ -6014,7 +6034,7 @@
       <c r="G12" s="125"/>
       <c r="H12" s="125"/>
     </row>
-    <row r="13" spans="2:12" ht="20" customHeight="1">
+    <row r="13" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B13" s="126">
         <v>4</v>
       </c>
@@ -6027,7 +6047,7 @@
       <c r="G13" s="125"/>
       <c r="H13" s="125"/>
     </row>
-    <row r="14" spans="2:12" ht="20" customHeight="1">
+    <row r="14" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B14" s="126">
         <v>5</v>
       </c>
@@ -6040,7 +6060,7 @@
       <c r="G14" s="125"/>
       <c r="H14" s="125"/>
     </row>
-    <row r="15" spans="2:12" ht="20" customHeight="1">
+    <row r="15" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B15" s="126">
         <v>6</v>
       </c>
@@ -6053,7 +6073,7 @@
       <c r="G15" s="125"/>
       <c r="H15" s="125"/>
     </row>
-    <row r="17" spans="2:8">
+    <row r="17" spans="2:8" ht="15.75">
       <c r="B17" s="123" t="s">
         <v>21</v>
       </c>
@@ -6061,22 +6081,22 @@
       <c r="D17" s="132"/>
       <c r="E17" s="122"/>
     </row>
-    <row r="18" spans="2:8">
+    <row r="18" spans="2:8" ht="15.75">
       <c r="B18" s="104" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="144" t="s">
         <v>231</v>
       </c>
-      <c r="D18" s="204" t="s">
+      <c r="D18" s="205" t="s">
         <v>234</v>
       </c>
-      <c r="E18" s="204"/>
+      <c r="E18" s="205"/>
       <c r="F18" s="144" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="20" customHeight="1">
+    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B19" s="126">
         <v>1</v>
       </c>
@@ -6089,7 +6109,7 @@
       <c r="G19" s="125"/>
       <c r="H19" s="125"/>
     </row>
-    <row r="20" spans="2:8" ht="20" customHeight="1">
+    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B20" s="126">
         <v>2</v>
       </c>
@@ -6102,7 +6122,7 @@
       <c r="G20" s="125"/>
       <c r="H20" s="125"/>
     </row>
-    <row r="21" spans="2:8" ht="20" customHeight="1">
+    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B21" s="126">
         <v>3</v>
       </c>
@@ -6115,7 +6135,7 @@
       <c r="G21" s="125"/>
       <c r="H21" s="125"/>
     </row>
-    <row r="22" spans="2:8" ht="20" customHeight="1">
+    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B22" s="126">
         <v>4</v>
       </c>
@@ -6128,7 +6148,7 @@
       <c r="G22" s="125"/>
       <c r="H22" s="125"/>
     </row>
-    <row r="23" spans="2:8" ht="20" customHeight="1">
+    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B23" s="126">
         <v>5</v>
       </c>
@@ -6141,7 +6161,7 @@
       <c r="G23" s="125"/>
       <c r="H23" s="125"/>
     </row>
-    <row r="24" spans="2:8" ht="20" customHeight="1">
+    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B24" s="126">
         <v>6</v>
       </c>
@@ -6154,7 +6174,7 @@
       <c r="G24" s="125"/>
       <c r="H24" s="125"/>
     </row>
-    <row r="26" spans="2:8">
+    <row r="26" spans="2:8" ht="15.75">
       <c r="B26" s="123" t="s">
         <v>233</v>
       </c>
@@ -6162,61 +6182,73 @@
       <c r="D26" s="132"/>
       <c r="E26" s="122"/>
     </row>
-    <row r="27" spans="2:8">
+    <row r="27" spans="2:8" ht="15.75">
       <c r="B27" s="104" t="s">
         <v>2</v>
       </c>
       <c r="C27" s="144" t="s">
         <v>231</v>
       </c>
-      <c r="D27" s="204" t="s">
+      <c r="D27" s="205" t="s">
         <v>234</v>
       </c>
-      <c r="E27" s="204"/>
+      <c r="E27" s="205"/>
       <c r="F27" s="144" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="20" customHeight="1">
+    <row r="28" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B28" s="147">
         <v>1</v>
       </c>
       <c r="C28" s="148" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="207"/>
-      <c r="E28" s="207"/>
-      <c r="F28" s="150"/>
+      <c r="D28" s="204" t="s">
+        <v>248</v>
+      </c>
+      <c r="E28" s="204"/>
+      <c r="F28" s="150" t="s">
+        <v>251</v>
+      </c>
       <c r="G28" s="125"/>
       <c r="H28" s="125"/>
     </row>
-    <row r="29" spans="2:8" ht="20" customHeight="1">
+    <row r="29" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B29" s="126">
         <v>2</v>
       </c>
       <c r="C29" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="203"/>
+      <c r="D29" s="203" t="s">
+        <v>249</v>
+      </c>
       <c r="E29" s="203"/>
-      <c r="F29" s="146"/>
+      <c r="F29" s="146" t="s">
+        <v>252</v>
+      </c>
       <c r="G29" s="125"/>
       <c r="H29" s="125"/>
     </row>
-    <row r="30" spans="2:8" ht="20" customHeight="1">
+    <row r="30" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B30" s="126">
         <v>3</v>
       </c>
       <c r="C30" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="203"/>
+      <c r="D30" s="203" t="s">
+        <v>250</v>
+      </c>
       <c r="E30" s="203"/>
-      <c r="F30" s="146"/>
+      <c r="F30" s="146" t="s">
+        <v>250</v>
+      </c>
       <c r="G30" s="125"/>
       <c r="H30" s="125"/>
     </row>
-    <row r="31" spans="2:8" ht="20" customHeight="1">
+    <row r="31" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B31" s="126">
         <v>4</v>
       </c>
@@ -6229,7 +6261,7 @@
       <c r="G31" s="125"/>
       <c r="H31" s="125"/>
     </row>
-    <row r="32" spans="2:8" ht="20" customHeight="1">
+    <row r="32" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B32" s="126">
         <v>5</v>
       </c>
@@ -6242,7 +6274,7 @@
       <c r="G32" s="125"/>
       <c r="H32" s="125"/>
     </row>
-    <row r="33" spans="2:8" ht="20" customHeight="1">
+    <row r="33" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B33" s="126">
         <v>6</v>
       </c>
@@ -6255,7 +6287,7 @@
       <c r="G33" s="125"/>
       <c r="H33" s="125"/>
     </row>
-    <row r="34" spans="2:8" ht="20" customHeight="1">
+    <row r="34" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B34" s="126">
         <v>7</v>
       </c>
@@ -6268,7 +6300,7 @@
       <c r="G34" s="125"/>
       <c r="H34" s="125"/>
     </row>
-    <row r="35" spans="2:8" ht="20" customHeight="1">
+    <row r="35" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B35" s="126">
         <v>8</v>
       </c>
@@ -6281,7 +6313,7 @@
       <c r="G35" s="125"/>
       <c r="H35" s="125"/>
     </row>
-    <row r="36" spans="2:8" ht="20" customHeight="1">
+    <row r="36" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B36" s="126">
         <v>9</v>
       </c>
@@ -6294,7 +6326,7 @@
       <c r="G36" s="125"/>
       <c r="H36" s="125"/>
     </row>
-    <row r="39" spans="2:8">
+    <row r="39" spans="2:8" ht="15.75">
       <c r="B39" s="123" t="s">
         <v>114</v>
       </c>
@@ -6302,15 +6334,15 @@
       <c r="D39" s="132"/>
       <c r="E39" s="122"/>
     </row>
-    <row r="40" spans="2:8">
+    <row r="40" spans="2:8" ht="15.75">
       <c r="B40" s="124"/>
       <c r="C40" s="157" t="s">
         <v>231</v>
       </c>
-      <c r="D40" s="204" t="s">
+      <c r="D40" s="205" t="s">
         <v>234</v>
       </c>
-      <c r="E40" s="204"/>
+      <c r="E40" s="205"/>
       <c r="F40" s="157" t="s">
         <v>232</v>
       </c>
@@ -6368,7 +6400,7 @@
       <c r="E45" s="203"/>
       <c r="F45" s="146"/>
     </row>
-    <row r="48" spans="2:8">
+    <row r="48" spans="2:8" ht="15.75">
       <c r="B48" s="123" t="s">
         <v>94</v>
       </c>
@@ -6376,20 +6408,20 @@
       <c r="D48" s="132"/>
       <c r="E48" s="122"/>
     </row>
-    <row r="49" spans="2:6">
+    <row r="49" spans="2:6" ht="15.75">
       <c r="B49" s="124"/>
       <c r="C49" s="144" t="s">
         <v>231</v>
       </c>
-      <c r="D49" s="204" t="s">
+      <c r="D49" s="205" t="s">
         <v>234</v>
       </c>
-      <c r="E49" s="204"/>
+      <c r="E49" s="205"/>
       <c r="F49" s="144" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="20" customHeight="1">
+    <row r="50" spans="2:6" ht="20.100000000000001" customHeight="1">
       <c r="B50" s="126">
         <v>1</v>
       </c>
@@ -6400,7 +6432,7 @@
       <c r="E50" s="203"/>
       <c r="F50" s="146"/>
     </row>
-    <row r="51" spans="2:6" ht="20" customHeight="1">
+    <row r="51" spans="2:6" ht="20.100000000000001" customHeight="1">
       <c r="B51" s="126">
         <v>2</v>
       </c>
@@ -6411,7 +6443,7 @@
       <c r="E51" s="203"/>
       <c r="F51" s="146"/>
     </row>
-    <row r="52" spans="2:6" ht="20" customHeight="1">
+    <row r="52" spans="2:6" ht="20.100000000000001" customHeight="1">
       <c r="B52" s="126">
         <v>3</v>
       </c>
@@ -6422,7 +6454,7 @@
       <c r="E52" s="203"/>
       <c r="F52" s="146"/>
     </row>
-    <row r="53" spans="2:6" ht="20" customHeight="1">
+    <row r="53" spans="2:6" ht="20.100000000000001" customHeight="1">
       <c r="B53" s="126">
         <v>4</v>
       </c>
@@ -6433,7 +6465,7 @@
       <c r="E53" s="203"/>
       <c r="F53" s="146"/>
     </row>
-    <row r="54" spans="2:6" ht="20" customHeight="1">
+    <row r="54" spans="2:6" ht="20.100000000000001" customHeight="1">
       <c r="B54" s="126">
         <v>5</v>
       </c>
@@ -6444,7 +6476,7 @@
       <c r="E54" s="203"/>
       <c r="F54" s="146"/>
     </row>
-    <row r="55" spans="2:6" ht="20" customHeight="1">
+    <row r="55" spans="2:6" ht="20.100000000000001" customHeight="1">
       <c r="B55" s="126">
         <v>6</v>
       </c>
@@ -6455,7 +6487,7 @@
       <c r="E55" s="203"/>
       <c r="F55" s="146"/>
     </row>
-    <row r="56" spans="2:6" ht="20" customHeight="1">
+    <row r="56" spans="2:6" ht="20.100000000000001" customHeight="1">
       <c r="B56" s="126">
         <v>7</v>
       </c>
@@ -6466,7 +6498,7 @@
       <c r="E56" s="203"/>
       <c r="F56" s="146"/>
     </row>
-    <row r="59" spans="2:6">
+    <row r="59" spans="2:6" ht="15.75">
       <c r="B59" s="123" t="s">
         <v>102</v>
       </c>
@@ -6474,15 +6506,15 @@
       <c r="D59" s="132"/>
       <c r="E59" s="122"/>
     </row>
-    <row r="60" spans="2:6">
+    <row r="60" spans="2:6" ht="15.75">
       <c r="B60" s="124"/>
       <c r="C60" s="144" t="s">
         <v>231</v>
       </c>
-      <c r="D60" s="204" t="s">
+      <c r="D60" s="205" t="s">
         <v>234</v>
       </c>
-      <c r="E60" s="204"/>
+      <c r="E60" s="205"/>
       <c r="F60" s="144" t="s">
         <v>232</v>
       </c>
@@ -6494,8 +6526,8 @@
       <c r="C61" s="127" t="s">
         <v>103</v>
       </c>
-      <c r="D61" s="205"/>
-      <c r="E61" s="206"/>
+      <c r="D61" s="206"/>
+      <c r="E61" s="207"/>
       <c r="F61" s="146"/>
     </row>
     <row r="62" spans="2:6" ht="15" customHeight="1">
@@ -6505,8 +6537,8 @@
       <c r="C62" s="127" t="s">
         <v>104</v>
       </c>
-      <c r="D62" s="205"/>
-      <c r="E62" s="206"/>
+      <c r="D62" s="206"/>
+      <c r="E62" s="207"/>
       <c r="F62" s="146"/>
     </row>
     <row r="63" spans="2:6" ht="15" customHeight="1">
@@ -6516,8 +6548,8 @@
       <c r="C63" s="127" t="s">
         <v>105</v>
       </c>
-      <c r="D63" s="205"/>
-      <c r="E63" s="206"/>
+      <c r="D63" s="206"/>
+      <c r="E63" s="207"/>
       <c r="F63" s="146"/>
     </row>
     <row r="64" spans="2:6" ht="15" customHeight="1">
@@ -6527,8 +6559,8 @@
       <c r="C64" s="127" t="s">
         <v>106</v>
       </c>
-      <c r="D64" s="205"/>
-      <c r="E64" s="206"/>
+      <c r="D64" s="206"/>
+      <c r="E64" s="207"/>
       <c r="F64" s="146"/>
     </row>
     <row r="65" spans="2:6">
@@ -6538,21 +6570,33 @@
       <c r="C65" s="127" t="s">
         <v>107</v>
       </c>
-      <c r="D65" s="205"/>
-      <c r="E65" s="206"/>
+      <c r="D65" s="206"/>
+      <c r="E65" s="207"/>
       <c r="F65" s="146"/>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
     <mergeCell ref="D64:E64"/>
     <mergeCell ref="D65:E65"/>
     <mergeCell ref="D23:E23"/>
@@ -6569,27 +6613,15 @@
     <mergeCell ref="D62:E62"/>
     <mergeCell ref="D53:E53"/>
     <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
   </mergeCells>
   <phoneticPr fontId="14"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6610,21 +6642,21 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.5" style="36" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" style="36" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" style="36" customWidth="1"/>
+    <col min="2" max="2" width="7.875" style="36" customWidth="1"/>
+    <col min="3" max="3" width="26.625" style="36" customWidth="1"/>
     <col min="4" max="4" width="11.5" style="36" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="36" customWidth="1"/>
-    <col min="6" max="6" width="48.6640625" style="36" customWidth="1"/>
-    <col min="7" max="7" width="62.33203125" style="36" customWidth="1"/>
-    <col min="8" max="8" width="62.83203125" style="36" customWidth="1"/>
+    <col min="5" max="5" width="10.625" style="36" customWidth="1"/>
+    <col min="6" max="6" width="48.625" style="36" customWidth="1"/>
+    <col min="7" max="7" width="62.375" style="36" customWidth="1"/>
+    <col min="8" max="8" width="62.875" style="36" customWidth="1"/>
     <col min="9" max="9" width="57.5" style="36" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="36"/>
+    <col min="10" max="16384" width="10.875" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" s="34" customFormat="1" ht="26" customHeight="1">
+    <row r="1" spans="2:14" s="34" customFormat="1" ht="26.1" customHeight="1">
       <c r="B1" s="133" t="s">
         <v>167</v>
       </c>
@@ -6681,7 +6713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="20" customHeight="1">
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1">
       <c r="B5" s="105">
         <v>1</v>
       </c>
@@ -6706,7 +6738,7 @@
       <c r="I5" s="110"/>
       <c r="J5" s="38"/>
     </row>
-    <row r="6" spans="2:14" ht="20" customHeight="1">
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1">
       <c r="B6" s="105">
         <v>2</v>
       </c>
@@ -6719,7 +6751,7 @@
       <c r="I6" s="110"/>
       <c r="J6" s="38"/>
     </row>
-    <row r="7" spans="2:14" ht="20" customHeight="1">
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1">
       <c r="B7" s="105">
         <v>3</v>
       </c>
@@ -6732,7 +6764,7 @@
       <c r="I7" s="110"/>
       <c r="J7" s="38"/>
     </row>
-    <row r="8" spans="2:14" ht="20" customHeight="1">
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1">
       <c r="B8" s="105">
         <v>4</v>
       </c>
@@ -6745,7 +6777,7 @@
       <c r="I8" s="110"/>
       <c r="J8" s="38"/>
     </row>
-    <row r="9" spans="2:14" ht="20" customHeight="1">
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1">
       <c r="B9" s="105">
         <v>5</v>
       </c>
@@ -6758,7 +6790,7 @@
       <c r="I9" s="110"/>
       <c r="J9" s="38"/>
     </row>
-    <row r="10" spans="2:14" ht="20" customHeight="1">
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1">
       <c r="B10" s="105">
         <v>6</v>
       </c>
@@ -6773,7 +6805,7 @@
       </c>
       <c r="J10" s="38"/>
     </row>
-    <row r="11" spans="2:14" ht="20" customHeight="1">
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1">
       <c r="B11" s="105">
         <v>7</v>
       </c>
@@ -6786,7 +6818,7 @@
       <c r="I11" s="110"/>
       <c r="J11" s="38"/>
     </row>
-    <row r="12" spans="2:14" ht="20" customHeight="1">
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1">
       <c r="B12" s="105">
         <v>8</v>
       </c>
@@ -6801,7 +6833,7 @@
       <c r="I12" s="110"/>
       <c r="J12" s="38"/>
     </row>
-    <row r="13" spans="2:14" ht="20" customHeight="1">
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1">
       <c r="B13" s="105">
         <v>9</v>
       </c>
@@ -6816,7 +6848,7 @@
       </c>
       <c r="J13" s="38"/>
     </row>
-    <row r="14" spans="2:14" ht="20" customHeight="1">
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1">
       <c r="B14" s="105">
         <v>10</v>
       </c>
@@ -6829,7 +6861,7 @@
       <c r="I14" s="110"/>
       <c r="J14" s="38"/>
     </row>
-    <row r="15" spans="2:14" ht="20" customHeight="1">
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1">
       <c r="B15" s="105">
         <v>11</v>
       </c>
@@ -6842,7 +6874,7 @@
       <c r="I15" s="110"/>
       <c r="J15" s="38"/>
     </row>
-    <row r="16" spans="2:14" ht="20" customHeight="1">
+    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1">
       <c r="B16" s="105">
         <v>12</v>
       </c>
@@ -6855,7 +6887,7 @@
       <c r="I16" s="110"/>
       <c r="J16" s="38"/>
     </row>
-    <row r="17" spans="2:10" ht="20" customHeight="1">
+    <row r="17" spans="2:10" ht="20.100000000000001" customHeight="1">
       <c r="B17" s="105">
         <v>13</v>
       </c>
@@ -6868,7 +6900,7 @@
       <c r="I17" s="110"/>
       <c r="J17" s="38"/>
     </row>
-    <row r="18" spans="2:10" ht="20" customHeight="1">
+    <row r="18" spans="2:10" ht="20.100000000000001" customHeight="1">
       <c r="B18" s="105">
         <v>14</v>
       </c>
@@ -6881,7 +6913,7 @@
       <c r="I18" s="110"/>
       <c r="J18" s="38"/>
     </row>
-    <row r="19" spans="2:10" ht="20" customHeight="1">
+    <row r="19" spans="2:10" ht="20.100000000000001" customHeight="1">
       <c r="B19" s="105">
         <v>15</v>
       </c>
@@ -6894,7 +6926,7 @@
       <c r="I19" s="110"/>
       <c r="J19" s="38"/>
     </row>
-    <row r="20" spans="2:10" ht="20" customHeight="1">
+    <row r="20" spans="2:10" ht="20.100000000000001" customHeight="1">
       <c r="B20" s="105">
         <v>16</v>
       </c>
@@ -6909,7 +6941,7 @@
       <c r="I20" s="110"/>
       <c r="J20" s="38"/>
     </row>
-    <row r="21" spans="2:10" ht="20" customHeight="1">
+    <row r="21" spans="2:10" ht="20.100000000000001" customHeight="1">
       <c r="B21" s="105">
         <v>17</v>
       </c>
@@ -6922,7 +6954,7 @@
       <c r="I21" s="110"/>
       <c r="J21" s="38"/>
     </row>
-    <row r="22" spans="2:10" ht="20" customHeight="1">
+    <row r="22" spans="2:10" ht="20.100000000000001" customHeight="1">
       <c r="B22" s="105">
         <v>18</v>
       </c>
@@ -6935,7 +6967,7 @@
       <c r="I22" s="110"/>
       <c r="J22" s="38"/>
     </row>
-    <row r="23" spans="2:10" ht="20" customHeight="1">
+    <row r="23" spans="2:10" ht="20.100000000000001" customHeight="1">
       <c r="B23" s="105">
         <v>19</v>
       </c>
@@ -6948,7 +6980,7 @@
       <c r="I23" s="110"/>
       <c r="J23" s="38"/>
     </row>
-    <row r="24" spans="2:10" ht="20" customHeight="1">
+    <row r="24" spans="2:10" ht="20.100000000000001" customHeight="1">
       <c r="B24" s="105">
         <v>20</v>
       </c>
@@ -6961,7 +6993,7 @@
       <c r="I24" s="110"/>
       <c r="J24" s="38"/>
     </row>
-    <row r="25" spans="2:10" ht="20" customHeight="1">
+    <row r="25" spans="2:10" ht="20.100000000000001" customHeight="1">
       <c r="B25" s="105">
         <v>21</v>
       </c>
@@ -6974,7 +7006,7 @@
       <c r="I25" s="110"/>
       <c r="J25" s="38"/>
     </row>
-    <row r="26" spans="2:10" ht="20" customHeight="1">
+    <row r="26" spans="2:10" ht="20.100000000000001" customHeight="1">
       <c r="B26" s="105">
         <v>22</v>
       </c>
@@ -6987,7 +7019,7 @@
       <c r="I26" s="110"/>
       <c r="J26" s="38"/>
     </row>
-    <row r="27" spans="2:10" ht="20" customHeight="1">
+    <row r="27" spans="2:10" ht="20.100000000000001" customHeight="1">
       <c r="B27" s="105">
         <v>23</v>
       </c>
@@ -7000,7 +7032,7 @@
       <c r="I27" s="110"/>
       <c r="J27" s="38"/>
     </row>
-    <row r="28" spans="2:10" ht="20" customHeight="1">
+    <row r="28" spans="2:10" ht="20.100000000000001" customHeight="1">
       <c r="B28" s="105">
         <v>24</v>
       </c>
@@ -7013,7 +7045,7 @@
       <c r="I28" s="110"/>
       <c r="J28" s="38"/>
     </row>
-    <row r="29" spans="2:10" ht="20" customHeight="1">
+    <row r="29" spans="2:10" ht="20.100000000000001" customHeight="1">
       <c r="B29" s="58"/>
       <c r="C29" s="65"/>
       <c r="D29" s="59"/>
@@ -7024,7 +7056,7 @@
       <c r="I29" s="61"/>
       <c r="J29" s="38"/>
     </row>
-    <row r="30" spans="2:10" ht="20" customHeight="1">
+    <row r="30" spans="2:10" ht="20.100000000000001" customHeight="1">
       <c r="B30" s="39"/>
       <c r="C30" s="64"/>
       <c r="D30" s="40"/>
@@ -7035,7 +7067,7 @@
       <c r="I30" s="61"/>
       <c r="J30" s="38"/>
     </row>
-    <row r="31" spans="2:10" ht="20" customHeight="1">
+    <row r="31" spans="2:10" ht="20.100000000000001" customHeight="1">
       <c r="B31" s="39"/>
       <c r="C31" s="64"/>
       <c r="D31" s="40"/>
@@ -7068,28 +7100,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A70" workbookViewId="0">
       <selection activeCell="L68" sqref="L68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="67"/>
-    <col min="2" max="2" width="17.83203125" style="67" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="67"/>
+    <col min="2" max="2" width="17.875" style="67" customWidth="1"/>
     <col min="3" max="3" width="15" style="67" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="67" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" style="67" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="67" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="67"/>
-    <col min="8" max="8" width="11.83203125" style="67" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.625" style="67" customWidth="1"/>
+    <col min="5" max="5" width="21.125" style="67" customWidth="1"/>
+    <col min="6" max="6" width="13.625" style="67" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.875" style="67"/>
+    <col min="8" max="8" width="11.875" style="67" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24" style="67" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.5" style="67" customWidth="1"/>
-    <col min="11" max="11" width="5.83203125" style="67" customWidth="1"/>
-    <col min="12" max="12" width="38.83203125" style="67" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="67"/>
+    <col min="11" max="11" width="5.875" style="67" customWidth="1"/>
+    <col min="12" max="12" width="38.875" style="67" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.875" style="67"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="20" customHeight="1">
+    <row r="1" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="66"/>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -7106,7 +7138,7 @@
       <c r="N1" s="66"/>
       <c r="O1" s="66"/>
     </row>
-    <row r="2" spans="1:15" ht="20" customHeight="1">
+    <row r="2" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="68" t="s">
         <v>142</v>
       </c>
@@ -7127,7 +7159,7 @@
       <c r="N2" s="66"/>
       <c r="O2" s="66"/>
     </row>
-    <row r="3" spans="1:15" ht="20" customHeight="1">
+    <row r="3" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="66"/>
       <c r="B3" s="69" t="s">
         <v>128</v>
@@ -7146,20 +7178,20 @@
       <c r="N3" s="66"/>
       <c r="O3" s="66"/>
     </row>
-    <row r="4" spans="1:15" ht="20" customHeight="1">
+    <row r="4" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="66"/>
       <c r="B4" s="70" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="218" t="s">
+      <c r="C4" s="220" t="s">
         <v>177</v>
       </c>
-      <c r="D4" s="219"/>
-      <c r="E4" s="219"/>
-      <c r="F4" s="219"/>
-      <c r="G4" s="219"/>
-      <c r="H4" s="219"/>
-      <c r="I4" s="220"/>
+      <c r="D4" s="230"/>
+      <c r="E4" s="230"/>
+      <c r="F4" s="230"/>
+      <c r="G4" s="230"/>
+      <c r="H4" s="230"/>
+      <c r="I4" s="219"/>
       <c r="J4" s="66"/>
       <c r="K4" s="66"/>
       <c r="L4" s="66"/>
@@ -7167,20 +7199,20 @@
       <c r="N4" s="66"/>
       <c r="O4" s="66"/>
     </row>
-    <row r="5" spans="1:15" ht="20" customHeight="1">
+    <row r="5" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="66"/>
       <c r="B5" s="70" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="218" t="s">
+      <c r="C5" s="220" t="s">
         <v>174</v>
       </c>
-      <c r="D5" s="219"/>
-      <c r="E5" s="219"/>
-      <c r="F5" s="219"/>
-      <c r="G5" s="219"/>
-      <c r="H5" s="219"/>
-      <c r="I5" s="220"/>
+      <c r="D5" s="230"/>
+      <c r="E5" s="230"/>
+      <c r="F5" s="230"/>
+      <c r="G5" s="230"/>
+      <c r="H5" s="230"/>
+      <c r="I5" s="219"/>
       <c r="J5" s="66"/>
       <c r="K5" s="66"/>
       <c r="L5" s="66"/>
@@ -7188,7 +7220,7 @@
       <c r="N5" s="66"/>
       <c r="O5" s="66"/>
     </row>
-    <row r="6" spans="1:15" ht="20" customHeight="1">
+    <row r="6" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="66"/>
       <c r="B6" s="70" t="s">
         <v>179</v>
@@ -7209,20 +7241,20 @@
       <c r="N6" s="66"/>
       <c r="O6" s="66"/>
     </row>
-    <row r="7" spans="1:15" ht="20" customHeight="1">
+    <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="66"/>
       <c r="B7" s="70" t="s">
         <v>191</v>
       </c>
-      <c r="C7" s="218" t="s">
+      <c r="C7" s="220" t="s">
         <v>171</v>
       </c>
-      <c r="D7" s="219"/>
-      <c r="E7" s="219"/>
-      <c r="F7" s="219"/>
-      <c r="G7" s="219"/>
-      <c r="H7" s="219"/>
-      <c r="I7" s="220"/>
+      <c r="D7" s="230"/>
+      <c r="E7" s="230"/>
+      <c r="F7" s="230"/>
+      <c r="G7" s="230"/>
+      <c r="H7" s="230"/>
+      <c r="I7" s="219"/>
       <c r="J7" s="66"/>
       <c r="K7" s="66"/>
       <c r="L7" s="66"/>
@@ -7230,7 +7262,7 @@
       <c r="N7" s="66"/>
       <c r="O7" s="66"/>
     </row>
-    <row r="8" spans="1:15" ht="20" customHeight="1">
+    <row r="8" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="66"/>
       <c r="B8" s="70" t="s">
         <v>192</v>
@@ -7251,20 +7283,20 @@
       <c r="N8" s="66"/>
       <c r="O8" s="66"/>
     </row>
-    <row r="9" spans="1:15" ht="20" customHeight="1">
+    <row r="9" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="66"/>
       <c r="B9" s="70" t="s">
         <v>225</v>
       </c>
-      <c r="C9" s="218" t="s">
+      <c r="C9" s="220" t="s">
         <v>226</v>
       </c>
-      <c r="D9" s="219"/>
-      <c r="E9" s="219"/>
-      <c r="F9" s="219"/>
-      <c r="G9" s="219"/>
-      <c r="H9" s="219"/>
-      <c r="I9" s="220"/>
+      <c r="D9" s="230"/>
+      <c r="E9" s="230"/>
+      <c r="F9" s="230"/>
+      <c r="G9" s="230"/>
+      <c r="H9" s="230"/>
+      <c r="I9" s="219"/>
       <c r="J9" s="66"/>
       <c r="K9" s="66"/>
       <c r="L9" s="66"/>
@@ -7272,7 +7304,7 @@
       <c r="N9" s="66"/>
       <c r="O9" s="66"/>
     </row>
-    <row r="10" spans="1:15" ht="20" customHeight="1">
+    <row r="10" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="66"/>
       <c r="B10" s="66"/>
       <c r="C10" s="66"/>
@@ -7289,7 +7321,7 @@
       <c r="N10" s="66"/>
       <c r="O10" s="66"/>
     </row>
-    <row r="11" spans="1:15" ht="20" customHeight="1">
+    <row r="11" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="66"/>
       <c r="B11" s="74" t="s">
         <v>190</v>
@@ -7308,7 +7340,7 @@
       <c r="N11" s="66"/>
       <c r="O11" s="66"/>
     </row>
-    <row r="12" spans="1:15" ht="20" customHeight="1">
+    <row r="12" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="66"/>
       <c r="B12" s="74"/>
       <c r="C12" s="74"/>
@@ -7325,26 +7357,26 @@
       <c r="N12" s="66"/>
       <c r="O12" s="66"/>
     </row>
-    <row r="13" spans="1:15" ht="20" customHeight="1">
+    <row r="13" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="66"/>
-      <c r="B13" s="227" t="s">
+      <c r="B13" s="226" t="s">
         <v>131</v>
       </c>
-      <c r="C13" s="228"/>
-      <c r="D13" s="228"/>
-      <c r="E13" s="228"/>
-      <c r="F13" s="228"/>
-      <c r="G13" s="228"/>
-      <c r="H13" s="228"/>
-      <c r="I13" s="228"/>
-      <c r="J13" s="228"/>
-      <c r="K13" s="228"/>
-      <c r="L13" s="229"/>
+      <c r="C13" s="227"/>
+      <c r="D13" s="227"/>
+      <c r="E13" s="227"/>
+      <c r="F13" s="227"/>
+      <c r="G13" s="227"/>
+      <c r="H13" s="227"/>
+      <c r="I13" s="227"/>
+      <c r="J13" s="227"/>
+      <c r="K13" s="227"/>
+      <c r="L13" s="228"/>
       <c r="M13" s="66"/>
       <c r="N13" s="66"/>
       <c r="O13" s="66"/>
     </row>
-    <row r="14" spans="1:15" ht="20" customHeight="1">
+    <row r="14" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="66"/>
       <c r="B14" s="75"/>
       <c r="C14" s="76" t="s">
@@ -7368,16 +7400,16 @@
       <c r="I14" s="76" t="s">
         <v>138</v>
       </c>
-      <c r="J14" s="221" t="s">
+      <c r="J14" s="235" t="s">
         <v>0</v>
       </c>
-      <c r="K14" s="221"/>
-      <c r="L14" s="221"/>
+      <c r="K14" s="235"/>
+      <c r="L14" s="235"/>
       <c r="M14" s="66"/>
       <c r="N14" s="66"/>
       <c r="O14" s="66"/>
     </row>
-    <row r="15" spans="1:15" ht="20" customHeight="1">
+    <row r="15" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="66"/>
       <c r="B15" s="77"/>
       <c r="C15" s="78" t="s">
@@ -7401,16 +7433,16 @@
       <c r="I15" s="81" t="s">
         <v>184</v>
       </c>
-      <c r="J15" s="230" t="s">
+      <c r="J15" s="229" t="s">
         <v>185</v>
       </c>
-      <c r="K15" s="230"/>
-      <c r="L15" s="230"/>
+      <c r="K15" s="229"/>
+      <c r="L15" s="229"/>
       <c r="M15" s="66"/>
       <c r="N15" s="66"/>
       <c r="O15" s="66"/>
     </row>
-    <row r="16" spans="1:15" ht="20" customHeight="1">
+    <row r="16" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="66"/>
       <c r="B16" s="77"/>
       <c r="C16" s="78" t="s">
@@ -7434,16 +7466,16 @@
       <c r="I16" s="81" t="s">
         <v>188</v>
       </c>
-      <c r="J16" s="230" t="s">
+      <c r="J16" s="229" t="s">
         <v>189</v>
       </c>
-      <c r="K16" s="230"/>
-      <c r="L16" s="230"/>
+      <c r="K16" s="229"/>
+      <c r="L16" s="229"/>
       <c r="M16" s="66"/>
       <c r="N16" s="66"/>
       <c r="O16" s="66"/>
     </row>
-    <row r="17" spans="1:15" ht="20" customHeight="1">
+    <row r="17" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="66"/>
       <c r="B17" s="77"/>
       <c r="C17" s="78" t="s">
@@ -7476,7 +7508,7 @@
       <c r="N17" s="66"/>
       <c r="O17" s="66"/>
     </row>
-    <row r="18" spans="1:15" ht="20" customHeight="1">
+    <row r="18" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="66"/>
       <c r="B18" s="77"/>
       <c r="C18" s="78" t="s">
@@ -7500,16 +7532,16 @@
       <c r="I18" s="79" t="s">
         <v>197</v>
       </c>
-      <c r="J18" s="218" t="s">
+      <c r="J18" s="220" t="s">
         <v>200</v>
       </c>
-      <c r="K18" s="219"/>
-      <c r="L18" s="220"/>
+      <c r="K18" s="230"/>
+      <c r="L18" s="219"/>
       <c r="M18" s="66"/>
       <c r="N18" s="66"/>
       <c r="O18" s="66"/>
     </row>
-    <row r="19" spans="1:15" ht="20" customHeight="1">
+    <row r="19" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="66"/>
       <c r="B19" s="82"/>
       <c r="C19" s="78" t="s">
@@ -7533,16 +7565,16 @@
       <c r="I19" s="83" t="s">
         <v>204</v>
       </c>
-      <c r="J19" s="218" t="s">
+      <c r="J19" s="220" t="s">
         <v>205</v>
       </c>
-      <c r="K19" s="219"/>
-      <c r="L19" s="220"/>
+      <c r="K19" s="230"/>
+      <c r="L19" s="219"/>
       <c r="M19" s="66"/>
       <c r="N19" s="66"/>
       <c r="O19" s="66"/>
     </row>
-    <row r="20" spans="1:15" ht="20" customHeight="1">
+    <row r="20" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="66"/>
       <c r="B20" s="84"/>
       <c r="C20" s="85"/>
@@ -7559,7 +7591,7 @@
       <c r="N20" s="66"/>
       <c r="O20" s="66"/>
     </row>
-    <row r="21" spans="1:15" ht="20" customHeight="1">
+    <row r="21" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="66"/>
       <c r="B21" s="74" t="s">
         <v>223</v>
@@ -7578,7 +7610,7 @@
       <c r="N21" s="66"/>
       <c r="O21" s="66"/>
     </row>
-    <row r="22" spans="1:15" ht="20" customHeight="1">
+    <row r="22" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="66"/>
       <c r="B22" s="84"/>
       <c r="C22" s="84"/>
@@ -7595,7 +7627,7 @@
       <c r="N22" s="66"/>
       <c r="O22" s="66"/>
     </row>
-    <row r="23" spans="1:15" ht="20" customHeight="1">
+    <row r="23" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="66"/>
       <c r="B23" s="84"/>
       <c r="C23" s="84"/>
@@ -7612,7 +7644,7 @@
       <c r="N23" s="66"/>
       <c r="O23" s="66"/>
     </row>
-    <row r="24" spans="1:15" ht="20" customHeight="1">
+    <row r="24" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="66"/>
       <c r="B24" s="84"/>
       <c r="C24" s="84"/>
@@ -7629,7 +7661,7 @@
       <c r="N24" s="66"/>
       <c r="O24" s="66"/>
     </row>
-    <row r="25" spans="1:15" ht="20" customHeight="1">
+    <row r="25" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="66"/>
       <c r="B25" s="84"/>
       <c r="C25" s="84"/>
@@ -7646,7 +7678,7 @@
       <c r="N25" s="66"/>
       <c r="O25" s="66"/>
     </row>
-    <row r="26" spans="1:15" ht="20" customHeight="1">
+    <row r="26" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="66"/>
       <c r="B26" s="84"/>
       <c r="C26" s="84"/>
@@ -7663,7 +7695,7 @@
       <c r="N26" s="66"/>
       <c r="O26" s="66"/>
     </row>
-    <row r="27" spans="1:15" ht="20" customHeight="1">
+    <row r="27" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="66"/>
       <c r="B27" s="84"/>
       <c r="C27" s="84"/>
@@ -7680,7 +7712,7 @@
       <c r="N27" s="66"/>
       <c r="O27" s="66"/>
     </row>
-    <row r="28" spans="1:15" ht="20" customHeight="1">
+    <row r="28" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="66"/>
       <c r="B28" s="84"/>
       <c r="C28" s="84"/>
@@ -7697,7 +7729,7 @@
       <c r="N28" s="66"/>
       <c r="O28" s="66"/>
     </row>
-    <row r="29" spans="1:15" s="89" customFormat="1" ht="20" customHeight="1">
+    <row r="29" spans="1:15" s="89" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="69"/>
       <c r="B29" s="231" t="s">
         <v>193</v>
@@ -7716,14 +7748,14 @@
       <c r="N29" s="69"/>
       <c r="O29" s="69"/>
     </row>
-    <row r="30" spans="1:15" s="91" customFormat="1" ht="20" customHeight="1">
+    <row r="30" spans="1:15" s="91" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="90"/>
-      <c r="B30" s="224" t="s">
+      <c r="B30" s="223" t="s">
         <v>133</v>
       </c>
-      <c r="C30" s="225"/>
-      <c r="D30" s="225"/>
-      <c r="E30" s="226"/>
+      <c r="C30" s="224"/>
+      <c r="D30" s="224"/>
+      <c r="E30" s="225"/>
       <c r="F30" s="76" t="s">
         <v>132</v>
       </c>
@@ -7749,7 +7781,7 @@
       <c r="N30" s="90"/>
       <c r="O30" s="90"/>
     </row>
-    <row r="31" spans="1:15" ht="20" customHeight="1">
+    <row r="31" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="66"/>
       <c r="B31" s="92" t="s">
         <v>147</v>
@@ -7780,7 +7812,7 @@
       <c r="N31" s="66"/>
       <c r="O31" s="66"/>
     </row>
-    <row r="32" spans="1:15" ht="20" customHeight="1">
+    <row r="32" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="66"/>
       <c r="B32" s="92"/>
       <c r="C32" s="95" t="s">
@@ -7811,14 +7843,14 @@
       <c r="N32" s="66"/>
       <c r="O32" s="66"/>
     </row>
-    <row r="33" spans="1:15" ht="20" customHeight="1">
+    <row r="33" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="66"/>
       <c r="B33" s="92"/>
       <c r="C33" s="97"/>
-      <c r="D33" s="218" t="s">
+      <c r="D33" s="220" t="s">
         <v>211</v>
       </c>
-      <c r="E33" s="220"/>
+      <c r="E33" s="219"/>
       <c r="F33" s="78" t="s">
         <v>148</v>
       </c>
@@ -7844,14 +7876,14 @@
       <c r="N33" s="66"/>
       <c r="O33" s="66"/>
     </row>
-    <row r="34" spans="1:15" ht="20" customHeight="1">
+    <row r="34" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="66"/>
       <c r="B34" s="92"/>
       <c r="C34" s="99"/>
-      <c r="D34" s="218" t="s">
+      <c r="D34" s="220" t="s">
         <v>212</v>
       </c>
-      <c r="E34" s="220"/>
+      <c r="E34" s="219"/>
       <c r="F34" s="78" t="s">
         <v>213</v>
       </c>
@@ -7877,7 +7909,7 @@
       <c r="N34" s="66"/>
       <c r="O34" s="66"/>
     </row>
-    <row r="35" spans="1:15" ht="20" customHeight="1">
+    <row r="35" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="66"/>
       <c r="B35" s="92"/>
       <c r="C35" s="95" t="s">
@@ -7910,14 +7942,14 @@
       <c r="N35" s="66"/>
       <c r="O35" s="66"/>
     </row>
-    <row r="36" spans="1:15" ht="20" customHeight="1">
+    <row r="36" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="66"/>
       <c r="B36" s="92"/>
       <c r="C36" s="102"/>
-      <c r="D36" s="218" t="s">
+      <c r="D36" s="220" t="s">
         <v>215</v>
       </c>
-      <c r="E36" s="220"/>
+      <c r="E36" s="219"/>
       <c r="F36" s="78" t="s">
         <v>217</v>
       </c>
@@ -7943,14 +7975,14 @@
       <c r="N36" s="66"/>
       <c r="O36" s="66"/>
     </row>
-    <row r="37" spans="1:15" ht="20" customHeight="1">
+    <row r="37" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="66"/>
       <c r="B37" s="92"/>
       <c r="C37" s="102"/>
-      <c r="D37" s="222" t="s">
+      <c r="D37" s="221" t="s">
         <v>181</v>
       </c>
-      <c r="E37" s="223"/>
+      <c r="E37" s="222"/>
       <c r="F37" s="78" t="s">
         <v>182</v>
       </c>
@@ -7976,14 +8008,14 @@
       <c r="N37" s="66"/>
       <c r="O37" s="66"/>
     </row>
-    <row r="38" spans="1:15" ht="20" customHeight="1">
+    <row r="38" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="66"/>
       <c r="B38" s="92"/>
       <c r="C38" s="97"/>
-      <c r="D38" s="218" t="s">
+      <c r="D38" s="220" t="s">
         <v>201</v>
       </c>
-      <c r="E38" s="220"/>
+      <c r="E38" s="219"/>
       <c r="F38" s="78" t="s">
         <v>194</v>
       </c>
@@ -8009,7 +8041,7 @@
       <c r="N38" s="66"/>
       <c r="O38" s="66"/>
     </row>
-    <row r="39" spans="1:15" ht="20" customHeight="1">
+    <row r="39" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="66"/>
       <c r="B39" s="92"/>
       <c r="C39" s="97"/>
@@ -8042,7 +8074,7 @@
       <c r="N39" s="66"/>
       <c r="O39" s="66"/>
     </row>
-    <row r="40" spans="1:15" ht="20" customHeight="1">
+    <row r="40" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="66"/>
       <c r="B40" s="92"/>
       <c r="C40" s="97"/>
@@ -8075,14 +8107,14 @@
       <c r="N40" s="66"/>
       <c r="O40" s="66"/>
     </row>
-    <row r="41" spans="1:15" ht="20" customHeight="1">
+    <row r="41" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="66"/>
       <c r="B41" s="98"/>
       <c r="C41" s="99"/>
-      <c r="D41" s="218" t="s">
+      <c r="D41" s="220" t="s">
         <v>149</v>
       </c>
-      <c r="E41" s="220"/>
+      <c r="E41" s="219"/>
       <c r="F41" s="78" t="s">
         <v>150</v>
       </c>
@@ -8108,7 +8140,7 @@
       <c r="N41" s="66"/>
       <c r="O41" s="66"/>
     </row>
-    <row r="42" spans="1:15" ht="20" customHeight="1">
+    <row r="42" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="66"/>
       <c r="B42" s="84"/>
       <c r="C42" s="93"/>
@@ -8125,7 +8157,7 @@
       <c r="N42" s="66"/>
       <c r="O42" s="66"/>
     </row>
-    <row r="43" spans="1:15" ht="20" customHeight="1">
+    <row r="43" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="66"/>
       <c r="B43" s="33" t="s">
         <v>228</v>
@@ -8144,7 +8176,7 @@
       <c r="N43" s="66"/>
       <c r="O43" s="66"/>
     </row>
-    <row r="44" spans="1:15" ht="20" customHeight="1">
+    <row r="44" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="66"/>
       <c r="B44" s="84"/>
       <c r="C44" s="93"/>
@@ -8161,7 +8193,7 @@
       <c r="N44" s="66"/>
       <c r="O44" s="66"/>
     </row>
-    <row r="45" spans="1:15" ht="20" customHeight="1">
+    <row r="45" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A45" s="66"/>
       <c r="B45" s="84"/>
       <c r="C45" s="93"/>
@@ -8178,7 +8210,7 @@
       <c r="N45" s="66"/>
       <c r="O45" s="66"/>
     </row>
-    <row r="46" spans="1:15" ht="20" customHeight="1">
+    <row r="46" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="66"/>
       <c r="B46" s="84"/>
       <c r="C46" s="93"/>
@@ -8195,7 +8227,7 @@
       <c r="N46" s="66"/>
       <c r="O46" s="66"/>
     </row>
-    <row r="47" spans="1:15" ht="20" customHeight="1">
+    <row r="47" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="66"/>
       <c r="B47" s="84"/>
       <c r="C47" s="93"/>
@@ -8212,7 +8244,7 @@
       <c r="N47" s="66"/>
       <c r="O47" s="66"/>
     </row>
-    <row r="48" spans="1:15" ht="20" customHeight="1">
+    <row r="48" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="66"/>
       <c r="B48" s="84"/>
       <c r="C48" s="93"/>
@@ -8229,7 +8261,7 @@
       <c r="N48" s="66"/>
       <c r="O48" s="66"/>
     </row>
-    <row r="49" spans="1:15" ht="20" customHeight="1">
+    <row r="49" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="66"/>
       <c r="B49" s="84"/>
       <c r="C49" s="93"/>
@@ -8246,7 +8278,7 @@
       <c r="N49" s="66"/>
       <c r="O49" s="66"/>
     </row>
-    <row r="50" spans="1:15" ht="20" customHeight="1">
+    <row r="50" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A50" s="66"/>
       <c r="B50" s="84"/>
       <c r="C50" s="93"/>
@@ -8263,7 +8295,7 @@
       <c r="N50" s="66"/>
       <c r="O50" s="66"/>
     </row>
-    <row r="51" spans="1:15" ht="20" customHeight="1">
+    <row r="51" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="66"/>
       <c r="B51" s="84"/>
       <c r="C51" s="93"/>
@@ -8280,7 +8312,7 @@
       <c r="N51" s="66"/>
       <c r="O51" s="66"/>
     </row>
-    <row r="52" spans="1:15" ht="20" customHeight="1">
+    <row r="52" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="66"/>
       <c r="B52" s="84"/>
       <c r="C52" s="93"/>
@@ -8297,7 +8329,7 @@
       <c r="N52" s="66"/>
       <c r="O52" s="66"/>
     </row>
-    <row r="53" spans="1:15" ht="20" customHeight="1">
+    <row r="53" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="66"/>
       <c r="B53" s="84"/>
       <c r="C53" s="93"/>
@@ -8314,7 +8346,7 @@
       <c r="N53" s="66"/>
       <c r="O53" s="66"/>
     </row>
-    <row r="54" spans="1:15" ht="20" customHeight="1">
+    <row r="54" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A54" s="66"/>
       <c r="B54" s="84"/>
       <c r="C54" s="93"/>
@@ -8331,7 +8363,7 @@
       <c r="N54" s="66"/>
       <c r="O54" s="66"/>
     </row>
-    <row r="55" spans="1:15" ht="20" customHeight="1">
+    <row r="55" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A55" s="66"/>
       <c r="B55" s="84"/>
       <c r="C55" s="93"/>
@@ -8348,7 +8380,7 @@
       <c r="N55" s="66"/>
       <c r="O55" s="66"/>
     </row>
-    <row r="56" spans="1:15" ht="20" customHeight="1">
+    <row r="56" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A56" s="66"/>
       <c r="B56" s="84"/>
       <c r="C56" s="93"/>
@@ -8365,7 +8397,7 @@
       <c r="N56" s="66"/>
       <c r="O56" s="66"/>
     </row>
-    <row r="57" spans="1:15" ht="20" customHeight="1">
+    <row r="57" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A57" s="66"/>
       <c r="B57" s="84"/>
       <c r="C57" s="93"/>
@@ -8382,7 +8414,7 @@
       <c r="N57" s="66"/>
       <c r="O57" s="66"/>
     </row>
-    <row r="58" spans="1:15" ht="20" customHeight="1">
+    <row r="58" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A58" s="66"/>
       <c r="B58" s="84"/>
       <c r="C58" s="93"/>
@@ -8399,7 +8431,7 @@
       <c r="N58" s="66"/>
       <c r="O58" s="66"/>
     </row>
-    <row r="59" spans="1:15" ht="20" customHeight="1">
+    <row r="59" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A59" s="66"/>
       <c r="B59" s="66"/>
       <c r="C59" s="66"/>
@@ -8416,7 +8448,7 @@
       <c r="N59" s="66"/>
       <c r="O59" s="66"/>
     </row>
-    <row r="60" spans="1:15" ht="20" customHeight="1">
+    <row r="60" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A60" s="66"/>
       <c r="B60" s="232" t="s">
         <v>152</v>
@@ -8437,14 +8469,14 @@
       <c r="N60" s="66"/>
       <c r="O60" s="66"/>
     </row>
-    <row r="61" spans="1:15" s="91" customFormat="1" ht="20" customHeight="1">
+    <row r="61" spans="1:15" s="91" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A61" s="90"/>
-      <c r="B61" s="224" t="s">
+      <c r="B61" s="223" t="s">
         <v>133</v>
       </c>
-      <c r="C61" s="225"/>
-      <c r="D61" s="225"/>
-      <c r="E61" s="226"/>
+      <c r="C61" s="224"/>
+      <c r="D61" s="224"/>
+      <c r="E61" s="225"/>
       <c r="F61" s="76" t="s">
         <v>132</v>
       </c>
@@ -8470,7 +8502,7 @@
       <c r="N61" s="90"/>
       <c r="O61" s="90"/>
     </row>
-    <row r="62" spans="1:15" ht="20" customHeight="1">
+    <row r="62" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A62" s="66"/>
       <c r="B62" s="92" t="s">
         <v>147</v>
@@ -8501,7 +8533,7 @@
       <c r="N62" s="66"/>
       <c r="O62" s="66"/>
     </row>
-    <row r="63" spans="1:15" ht="20" customHeight="1">
+    <row r="63" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A63" s="66"/>
       <c r="B63" s="92"/>
       <c r="C63" s="95" t="s">
@@ -8532,14 +8564,14 @@
       <c r="N63" s="66"/>
       <c r="O63" s="66"/>
     </row>
-    <row r="64" spans="1:15" ht="20" customHeight="1">
+    <row r="64" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A64" s="66"/>
       <c r="B64" s="92"/>
       <c r="C64" s="97"/>
-      <c r="D64" s="233" t="s">
+      <c r="D64" s="218" t="s">
         <v>211</v>
       </c>
-      <c r="E64" s="220"/>
+      <c r="E64" s="219"/>
       <c r="F64" s="78" t="s">
         <v>148</v>
       </c>
@@ -8565,14 +8597,14 @@
       <c r="N64" s="66"/>
       <c r="O64" s="66"/>
     </row>
-    <row r="65" spans="1:15" ht="20" customHeight="1">
+    <row r="65" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A65" s="66"/>
       <c r="B65" s="92"/>
       <c r="C65" s="97"/>
-      <c r="D65" s="233" t="s">
+      <c r="D65" s="218" t="s">
         <v>0</v>
       </c>
-      <c r="E65" s="234"/>
+      <c r="E65" s="233"/>
       <c r="F65" s="151" t="s">
         <v>237</v>
       </c>
@@ -8598,14 +8630,14 @@
       <c r="N65" s="66"/>
       <c r="O65" s="66"/>
     </row>
-    <row r="66" spans="1:15" ht="20" customHeight="1">
+    <row r="66" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A66" s="66"/>
       <c r="B66" s="92"/>
       <c r="C66" s="97"/>
-      <c r="D66" s="235" t="s">
+      <c r="D66" s="234" t="s">
         <v>242</v>
       </c>
-      <c r="E66" s="234"/>
+      <c r="E66" s="233"/>
       <c r="F66" s="151" t="s">
         <v>240</v>
       </c>
@@ -8631,7 +8663,7 @@
       <c r="N66" s="66"/>
       <c r="O66" s="66"/>
     </row>
-    <row r="67" spans="1:15" ht="20" customHeight="1">
+    <row r="67" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A67" s="66"/>
       <c r="B67" s="92"/>
       <c r="C67" s="102"/>
@@ -8664,7 +8696,7 @@
       <c r="N67" s="66"/>
       <c r="O67" s="66"/>
     </row>
-    <row r="68" spans="1:15" ht="20" customHeight="1">
+    <row r="68" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A68" s="66"/>
       <c r="B68" s="92"/>
       <c r="C68" s="95" t="s">
@@ -8695,12 +8727,12 @@
       <c r="N68" s="66"/>
       <c r="O68" s="66"/>
     </row>
-    <row r="69" spans="1:15" ht="20" customHeight="1">
+    <row r="69" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A69" s="66"/>
       <c r="B69" s="98"/>
       <c r="C69" s="99"/>
-      <c r="D69" s="218"/>
-      <c r="E69" s="220"/>
+      <c r="D69" s="220"/>
+      <c r="E69" s="219"/>
       <c r="F69" s="78"/>
       <c r="G69" s="80"/>
       <c r="H69" s="80"/>
@@ -8712,7 +8744,7 @@
       <c r="N69" s="66"/>
       <c r="O69" s="66"/>
     </row>
-    <row r="70" spans="1:15" ht="20" customHeight="1">
+    <row r="70" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A70" s="66"/>
       <c r="B70" s="84"/>
       <c r="C70" s="93"/>
@@ -8729,7 +8761,7 @@
       <c r="N70" s="66"/>
       <c r="O70" s="66"/>
     </row>
-    <row r="71" spans="1:15" ht="20" customHeight="1">
+    <row r="71" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A71" s="66"/>
       <c r="B71" s="74" t="s">
         <v>224</v>
@@ -8748,7 +8780,7 @@
       <c r="N71" s="66"/>
       <c r="O71" s="66"/>
     </row>
-    <row r="72" spans="1:15" ht="20" customHeight="1">
+    <row r="72" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A72" s="66"/>
       <c r="B72" s="66"/>
       <c r="C72" s="66"/>
@@ -8765,7 +8797,7 @@
       <c r="N72" s="66"/>
       <c r="O72" s="66"/>
     </row>
-    <row r="73" spans="1:15" ht="20" customHeight="1">
+    <row r="73" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A73" s="66"/>
       <c r="B73" s="66"/>
       <c r="C73" s="66"/>
@@ -8782,7 +8814,7 @@
       <c r="N73" s="66"/>
       <c r="O73" s="66"/>
     </row>
-    <row r="74" spans="1:15" ht="20" customHeight="1">
+    <row r="74" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A74" s="66"/>
       <c r="B74" s="66"/>
       <c r="C74" s="66"/>
@@ -8799,7 +8831,7 @@
       <c r="N74" s="66"/>
       <c r="O74" s="66"/>
     </row>
-    <row r="75" spans="1:15" ht="20" customHeight="1">
+    <row r="75" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A75" s="66"/>
       <c r="B75" s="66"/>
       <c r="C75" s="66"/>
@@ -8816,7 +8848,7 @@
       <c r="N75" s="66"/>
       <c r="O75" s="66"/>
     </row>
-    <row r="76" spans="1:15" ht="20" customHeight="1">
+    <row r="76" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A76" s="66"/>
       <c r="B76" s="66"/>
       <c r="C76" s="66"/>
@@ -8833,7 +8865,7 @@
       <c r="N76" s="66"/>
       <c r="O76" s="66"/>
     </row>
-    <row r="77" spans="1:15" ht="20" customHeight="1">
+    <row r="77" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A77" s="66"/>
       <c r="B77" s="66"/>
       <c r="C77" s="66"/>
@@ -8850,7 +8882,7 @@
       <c r="N77" s="66"/>
       <c r="O77" s="66"/>
     </row>
-    <row r="78" spans="1:15" ht="20" customHeight="1">
+    <row r="78" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A78" s="66"/>
       <c r="B78" s="66"/>
       <c r="C78" s="66"/>
@@ -8867,7 +8899,7 @@
       <c r="N78" s="66"/>
       <c r="O78" s="66"/>
     </row>
-    <row r="79" spans="1:15" ht="20" customHeight="1">
+    <row r="79" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A79" s="66"/>
       <c r="B79" s="66"/>
       <c r="C79" s="66"/>
@@ -8884,7 +8916,7 @@
       <c r="N79" s="66"/>
       <c r="O79" s="66"/>
     </row>
-    <row r="80" spans="1:15" ht="20" customHeight="1">
+    <row r="80" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A80" s="66"/>
       <c r="B80" s="66"/>
       <c r="C80" s="66"/>
@@ -8901,7 +8933,7 @@
       <c r="N80" s="66"/>
       <c r="O80" s="66"/>
     </row>
-    <row r="81" spans="1:15" ht="20" customHeight="1">
+    <row r="81" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A81" s="66"/>
       <c r="B81" s="66"/>
       <c r="C81" s="66"/>
@@ -8918,7 +8950,7 @@
       <c r="N81" s="66"/>
       <c r="O81" s="66"/>
     </row>
-    <row r="82" spans="1:15" ht="20" customHeight="1">
+    <row r="82" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A82" s="66"/>
       <c r="B82" s="66"/>
       <c r="C82" s="66"/>
@@ -8935,7 +8967,7 @@
       <c r="N82" s="66"/>
       <c r="O82" s="66"/>
     </row>
-    <row r="83" spans="1:15" ht="20" customHeight="1">
+    <row r="83" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A83" s="66"/>
       <c r="B83" s="66"/>
       <c r="C83" s="66"/>
@@ -8952,7 +8984,7 @@
       <c r="N83" s="66"/>
       <c r="O83" s="66"/>
     </row>
-    <row r="84" spans="1:15" ht="20" customHeight="1">
+    <row r="84" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A84" s="66"/>
       <c r="B84" s="66"/>
       <c r="C84" s="66"/>
@@ -8969,7 +9001,7 @@
       <c r="N84" s="66"/>
       <c r="O84" s="66"/>
     </row>
-    <row r="85" spans="1:15" ht="20" customHeight="1">
+    <row r="85" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A85" s="66"/>
       <c r="B85" s="66"/>
       <c r="C85" s="66"/>
@@ -8986,7 +9018,7 @@
       <c r="N85" s="66"/>
       <c r="O85" s="66"/>
     </row>
-    <row r="86" spans="1:15" ht="20" customHeight="1">
+    <row r="86" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A86" s="66"/>
       <c r="B86" s="66"/>
       <c r="C86" s="66"/>
@@ -9003,7 +9035,7 @@
       <c r="N86" s="66"/>
       <c r="O86" s="66"/>
     </row>
-    <row r="87" spans="1:15" ht="20" customHeight="1">
+    <row r="87" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A87" s="66"/>
       <c r="B87" s="66"/>
       <c r="C87" s="66"/>
@@ -9020,7 +9052,7 @@
       <c r="N87" s="66"/>
       <c r="O87" s="66"/>
     </row>
-    <row r="88" spans="1:15" ht="20" customHeight="1">
+    <row r="88" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A88" s="66"/>
       <c r="B88" s="66"/>
       <c r="C88" s="66"/>
@@ -9037,7 +9069,7 @@
       <c r="N88" s="66"/>
       <c r="O88" s="66"/>
     </row>
-    <row r="89" spans="1:15" ht="20" customHeight="1">
+    <row r="89" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A89" s="66"/>
       <c r="B89" s="66"/>
       <c r="C89" s="66"/>
@@ -9054,7 +9086,7 @@
       <c r="N89" s="66"/>
       <c r="O89" s="66"/>
     </row>
-    <row r="90" spans="1:15" ht="20" customHeight="1">
+    <row r="90" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A90" s="66"/>
       <c r="B90" s="66"/>
       <c r="C90" s="66"/>
@@ -9071,7 +9103,7 @@
       <c r="N90" s="66"/>
       <c r="O90" s="66"/>
     </row>
-    <row r="91" spans="1:15" ht="20" customHeight="1">
+    <row r="91" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A91" s="101"/>
       <c r="B91" s="101"/>
       <c r="C91" s="101"/>
@@ -9090,12 +9122,11 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="J14:L14"/>
     <mergeCell ref="D69:E69"/>
     <mergeCell ref="B13:L13"/>
     <mergeCell ref="B30:E30"/>
@@ -9109,11 +9140,12 @@
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="D65:E65"/>
     <mergeCell ref="D66:E66"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="B61:E61"/>
   </mergeCells>
   <phoneticPr fontId="14"/>
   <hyperlinks>

</xml_diff>